<commit_message>
unique modules, filtering out outlier driven correlations
</commit_message>
<xml_diff>
--- a/data/column_descriptors_standardized_101823.xlsx
+++ b/data/column_descriptors_standardized_101823.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="733">
   <si>
     <t xml:space="preserve">column_ID</t>
   </si>
@@ -2533,14 +2533,14 @@
   <dimension ref="A1:AU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A126" activeCellId="0" sqref="A126"/>
-      <selection pane="bottomRight" activeCell="C142" activeCellId="0" sqref="C142"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="J64" activeCellId="0" sqref="J64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.33"/>
@@ -8120,9 +8120,7 @@
       <c r="I63" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="J63" s="5" t="s">
-        <v>337</v>
-      </c>
+      <c r="J63" s="5"/>
       <c r="K63" s="5" t="s">
         <v>337</v>
       </c>
@@ -8213,9 +8211,7 @@
       <c r="I64" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="J64" s="5" t="s">
-        <v>337</v>
-      </c>
+      <c r="J64" s="5"/>
       <c r="K64" s="5" t="s">
         <v>337</v>
       </c>

</xml_diff>